<commit_message>
added raw material and part number details
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/05-BulkUploadRawMaterialType.xlsx
+++ b/documents/templates/bulk-upload/05-BulkUploadRawMaterialType.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BD9894-CB67-444A-9493-9228362DB6DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE037C0-4A58-F442-A4D5-50C0F95866B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{2EDA8A97-5D5A-9541-97ED-8ED17C0189D2}"/>
   </bookViews>
@@ -31,18 +31,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Profile</t>
   </si>
   <si>
     <t>Sheet</t>
   </si>
   <si>
-    <t>Pipe</t>
+    <t>Tube</t>
   </si>
 </sst>
 </file>
@@ -394,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1DD87E-4D9A-5441-AADE-3D991F0F269C}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,11 +414,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>